<commit_message>
updated control objectives and controls (ISO420001)t
</commit_message>
<xml_diff>
--- a/emerging technologies/artificial intelligence/Controls objectives and controls (AIMS_ISO42001).xlsx
+++ b/emerging technologies/artificial intelligence/Controls objectives and controls (AIMS_ISO42001).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">A.2 Policies related to AI </t>
   </si>
@@ -69,6 +69,120 @@
   </si>
   <si>
     <t xml:space="preserve">Table A.1 - Control objectives and controls </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.3 Internal organization </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective: To establish accountability within the organization to uphold its responsible approach for the implementation, operation and management of AI systems </t>
+  </si>
+  <si>
+    <t>A.3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI roles and responsibilities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roles abd responsibilities for AI shall be defined and allocated according to the needs of the organization </t>
+  </si>
+  <si>
+    <t>A.3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reporting of concerns </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The organzation shall define and put in place a process to report concerns about the organization's role with respect to an AI system throughout its life cycle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.4 Resources for AI systems </t>
+  </si>
+  <si>
+    <t>A.4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource documentation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The organization shall identify and document relevant resources required for the activities at given AI system life cycle stages and other AI-related activites relevant for the organization </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Resources </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As part of resource identification, the organization shall document information about the data resources uutilized for the AI system </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tooling resources </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As part of resource identification, the organization shall document information about the tooling resources utilized for the AI system </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System and computing resources </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As part of resource identification, the organization shall document information about the system and computing resources utilized for the AI system. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human resources </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As part of resource identification, the organization shall document information about the human resources and their competences utilized for the development, deployment, operation, change management, maintenance, transfer and decomissioning, as well as verification and integration of the AI system </t>
+  </si>
+  <si>
+    <t>A.4.3</t>
+  </si>
+  <si>
+    <t>A.4.4</t>
+  </si>
+  <si>
+    <t>A.4.5</t>
+  </si>
+  <si>
+    <t>A.4.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.5 Assessing impacts of AI systems </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective: To assess AI system impacts to individuals or groups of individuals or both, and societies affected by the AI system throughout its lifecycle </t>
+  </si>
+  <si>
+    <t>A.5.2</t>
+  </si>
+  <si>
+    <t>AI system impact assessment process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The organization shall establish a process to assess the potential consequences for individuals or groups of individuals, or both, and societies that can result from the AI system throughout its life cycle </t>
+  </si>
+  <si>
+    <t>A.5.3</t>
+  </si>
+  <si>
+    <t>A.5.4</t>
+  </si>
+  <si>
+    <t>A.5.5</t>
+  </si>
+  <si>
+    <t>Documentation of AI system impacts assessments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assessing AI systems impact on individuals or groups </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assessing societal impacts of AI systems </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The organization shall document the results of AI system impact assessments and retain results for a defined period </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The organization shall assess and document the potential impacts of AI systems to individuals throughout the systems lifecycle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The organization shall assess and document the potential societal impacts of their AI systems throughout their lifecycle </t>
   </si>
 </sst>
 </file>
@@ -398,15 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="52.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -469,6 +583,152 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>